<commit_message>
Suppression élément NODE.JS 6d5f846aba8dbd3eb1730bf1f5f99f4626eb7762
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/ValueSet-Laterality.xlsx
+++ b/update-mapping-pn13/ig/ValueSet-Laterality.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from Unified Medical " r:id="rId4" sheetId="2"/>
+    <sheet name="Include #0" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-30T13:12:38+00:00</t>
+    <t>2024-09-10T09:55:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>